<commit_message>
The SR phase now uses the specified stimulation order.
Signed-off-by: Julian-Webb <julian.webb00@gmail.com>
</commit_message>
<xml_diff>
--- a/data/test_stim_order.xlsx
+++ b/data/test_stim_order.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\PycharmProjects\EvokingSensation\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{267CE361-A41C-4C29-80F5-41D191595B5D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="StimulationOrder" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -28,12 +34,6 @@
     <t>electrodes</t>
   </si>
   <si>
-    <t>Overall trial</t>
-  </si>
-  <si>
-    <t>[7, 3, 1, 2, 4, 5, 6, 8]</t>
-  </si>
-  <si>
     <t>[1, 8, 6, 5, 4, 7, 3]</t>
   </si>
   <si>
@@ -127,9 +127,6 @@
     <t>[4, 8, 3]</t>
   </si>
   <si>
-    <t>[(13, 14), (5, 6), (1, 2), (3, 4), (7, 8), (9, 10), (11, 12), (15, 16)]</t>
-  </si>
-  <si>
     <t>[(1, 2), (15, 16), (11, 12), (9, 10), (7, 8), (13, 14), (5, 6)]</t>
   </si>
   <si>
@@ -221,13 +218,22 @@
   </si>
   <si>
     <t>[(7, 8), (15, 16), (5, 6)]</t>
+  </si>
+  <si>
+    <t>overall trial</t>
+  </si>
+  <si>
+    <t>[1, 2]</t>
+  </si>
+  <si>
+    <t>[(1, 2), (3, 4)]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -304,6 +310,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -350,7 +364,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -382,9 +396,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -416,6 +448,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -591,104 +641,106 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="5.85546875" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" customWidth="1"/>
-    <col min="5" max="5" width="71.85546875" customWidth="1"/>
+    <col min="2" max="3" width="5.88671875" customWidth="1"/>
+    <col min="4" max="4" width="24.88671875" customWidth="1"/>
+    <col min="5" max="5" width="71.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="E3" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E4" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2">
+        <v>3</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0</v>
-      </c>
-      <c r="C4" s="2">
-        <v>2</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2">
-        <v>3</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -699,13 +751,13 @@
         <v>4</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -716,13 +768,13 @@
         <v>5</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -733,13 +785,13 @@
         <v>6</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -750,13 +802,13 @@
         <v>7</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -767,13 +819,13 @@
         <v>0</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -784,13 +836,13 @@
         <v>1</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -801,13 +853,13 @@
         <v>2</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -818,13 +870,13 @@
         <v>3</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -835,13 +887,13 @@
         <v>4</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -852,13 +904,13 @@
         <v>5</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -869,13 +921,13 @@
         <v>6</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -886,13 +938,13 @@
         <v>7</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -903,13 +955,13 @@
         <v>0</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -920,13 +972,13 @@
         <v>1</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -937,13 +989,13 @@
         <v>2</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -954,13 +1006,13 @@
         <v>3</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -971,13 +1023,13 @@
         <v>4</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -988,13 +1040,13 @@
         <v>5</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1005,13 +1057,13 @@
         <v>6</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1022,13 +1074,13 @@
         <v>7</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1039,13 +1091,13 @@
         <v>0</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1056,13 +1108,13 @@
         <v>1</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1073,13 +1125,13 @@
         <v>2</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1090,13 +1142,13 @@
         <v>3</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1107,13 +1159,13 @@
         <v>4</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1124,13 +1176,13 @@
         <v>5</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1141,13 +1193,13 @@
         <v>6</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1158,10 +1210,10 @@
         <v>7</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>